<commit_message>
Finished Debugging for now ready for merge and gui work
</commit_message>
<xml_diff>
--- a/Shipping Excel Sheet Test.xlsx
+++ b/Shipping Excel Sheet Test.xlsx
@@ -600,9 +600,9 @@
           <t>CMAU0459057</t>
         </is>
       </c>
-      <c r="C2" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2022</t>
+      <c r="C2" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -617,9 +617,9 @@
           <t>CMAU1999430</t>
         </is>
       </c>
-      <c r="C3" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2023</t>
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>Date Error</t>
         </is>
       </c>
     </row>
@@ -634,9 +634,9 @@
           <t>TEMU1001882</t>
         </is>
       </c>
-      <c r="C4" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2024</t>
+      <c r="C4" s="17" t="inlineStr">
+        <is>
+          <t>Date Error</t>
         </is>
       </c>
     </row>
@@ -651,9 +651,9 @@
           <t>CMAU3124870</t>
         </is>
       </c>
-      <c r="C5" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2025</t>
+      <c r="C5" s="18" t="inlineStr">
+        <is>
+          <t>07/06/2022</t>
         </is>
       </c>
     </row>
@@ -668,9 +668,9 @@
           <t>CMAU1271001</t>
         </is>
       </c>
-      <c r="C6" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2026</t>
+      <c r="C6" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -685,9 +685,9 @@
           <t>CMAU1084274</t>
         </is>
       </c>
-      <c r="C7" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2027</t>
+      <c r="C7" s="18" t="inlineStr">
+        <is>
+          <t>07/07/2022</t>
         </is>
       </c>
     </row>
@@ -702,9 +702,9 @@
           <t>TLLU2340963</t>
         </is>
       </c>
-      <c r="C8" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2028</t>
+      <c r="C8" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -719,9 +719,9 @@
           <t>CMAU0786511</t>
         </is>
       </c>
-      <c r="C9" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2029</t>
+      <c r="C9" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -736,9 +736,9 @@
           <t>TGHU9843127</t>
         </is>
       </c>
-      <c r="C10" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2030</t>
+      <c r="C10" s="18" t="inlineStr">
+        <is>
+          <t>07/06/2022</t>
         </is>
       </c>
     </row>
@@ -753,9 +753,9 @@
           <t>BMOU2183772</t>
         </is>
       </c>
-      <c r="C11" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2031</t>
+      <c r="C11" s="17" t="inlineStr">
+        <is>
+          <t>Date Error</t>
         </is>
       </c>
     </row>
@@ -770,9 +770,9 @@
           <t>BMOU2182267</t>
         </is>
       </c>
-      <c r="C12" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2032</t>
+      <c r="C12" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -787,9 +787,9 @@
           <t>TEMU2454266</t>
         </is>
       </c>
-      <c r="C13" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2033</t>
+      <c r="C13" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
       <c r="F13" s="1" t="n"/>
@@ -805,9 +805,9 @@
           <t>CMAU0615186</t>
         </is>
       </c>
-      <c r="C14" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2034</t>
+      <c r="C14" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
       <c r="F14" s="1" t="n"/>
@@ -823,9 +823,9 @@
           <t>CMAU1671749</t>
         </is>
       </c>
-      <c r="C15" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2035</t>
+      <c r="C15" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
       <c r="F15" s="1" t="n"/>
@@ -841,9 +841,9 @@
           <t>FWRU0143517</t>
         </is>
       </c>
-      <c r="C16" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2036</t>
+      <c r="C16" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -858,9 +858,9 @@
           <t>TCLU9637873</t>
         </is>
       </c>
-      <c r="C17" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2037</t>
+      <c r="C17" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -875,9 +875,9 @@
           <t>TRHU6017442</t>
         </is>
       </c>
-      <c r="C18" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2038</t>
+      <c r="C18" s="18" t="inlineStr">
+        <is>
+          <t>07/17/2022</t>
         </is>
       </c>
     </row>
@@ -892,9 +892,9 @@
           <t>FCIU9357391</t>
         </is>
       </c>
-      <c r="C19" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2039</t>
+      <c r="C19" s="18" t="inlineStr">
+        <is>
+          <t>07/29/2022</t>
         </is>
       </c>
     </row>
@@ -909,9 +909,9 @@
           <t>CMAU7146898</t>
         </is>
       </c>
-      <c r="C20" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2040</t>
+      <c r="C20" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -926,9 +926,9 @@
           <t>CMAU5249433</t>
         </is>
       </c>
-      <c r="C21" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2041</t>
+      <c r="C21" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -943,9 +943,9 @@
           <t>CMAU5905357</t>
         </is>
       </c>
-      <c r="C22" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2042</t>
+      <c r="C22" s="18" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
         </is>
       </c>
     </row>
@@ -960,9 +960,9 @@
           <t>TGHU3892802</t>
         </is>
       </c>
-      <c r="C23" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2043</t>
+      <c r="C23" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -977,9 +977,9 @@
           <t>TGHU0157086</t>
         </is>
       </c>
-      <c r="C24" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2044</t>
+      <c r="C24" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -994,9 +994,9 @@
           <t>APZU3448600</t>
         </is>
       </c>
-      <c r="C25" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2045</t>
+      <c r="C25" s="18" t="inlineStr">
+        <is>
+          <t>07/05/2022</t>
         </is>
       </c>
     </row>
@@ -1011,9 +1011,9 @@
           <t>APZU3431438</t>
         </is>
       </c>
-      <c r="C26" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2046</t>
+      <c r="C26" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1028,9 +1028,9 @@
           <t>MAGU5474162</t>
         </is>
       </c>
-      <c r="C27" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2047</t>
+      <c r="C27" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1045,9 +1045,9 @@
           <t>TRLU6706305</t>
         </is>
       </c>
-      <c r="C28" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2048</t>
+      <c r="C28" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1062,9 +1062,9 @@
           <t>FCIU8749361</t>
         </is>
       </c>
-      <c r="C29" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2049</t>
+      <c r="C29" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1079,9 +1079,9 @@
           <t>CMAU5084396</t>
         </is>
       </c>
-      <c r="C30" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2050</t>
+      <c r="C30" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1096,9 +1096,9 @@
           <t>TCKU6331265</t>
         </is>
       </c>
-      <c r="C31" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2051</t>
+      <c r="C31" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1113,9 +1113,9 @@
           <t>TCNU2838050</t>
         </is>
       </c>
-      <c r="C32" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2052</t>
+      <c r="C32" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1130,9 +1130,9 @@
           <t>TEMU6960719</t>
         </is>
       </c>
-      <c r="C33" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2053</t>
+      <c r="C33" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1147,9 +1147,9 @@
           <t>TLLU4514961</t>
         </is>
       </c>
-      <c r="C34" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2054</t>
+      <c r="C34" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1164,9 +1164,9 @@
           <t>CMAU0594020</t>
         </is>
       </c>
-      <c r="C35" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2055</t>
+      <c r="C35" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1181,9 +1181,9 @@
           <t>CMAU1317484</t>
         </is>
       </c>
-      <c r="C36" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2056</t>
+      <c r="C36" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1198,9 +1198,9 @@
           <t>TCLU9647362</t>
         </is>
       </c>
-      <c r="C37" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2057</t>
+      <c r="C37" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1215,9 +1215,9 @@
           <t>TRHU8141283</t>
         </is>
       </c>
-      <c r="C38" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2058</t>
+      <c r="C38" s="18" t="inlineStr">
+        <is>
+          <t>08/04/2022</t>
         </is>
       </c>
     </row>
@@ -1232,9 +1232,9 @@
           <t>TCLU8644395</t>
         </is>
       </c>
-      <c r="C39" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2059</t>
+      <c r="C39" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1249,9 +1249,9 @@
           <t>JXLU7831639</t>
         </is>
       </c>
-      <c r="C40" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2060</t>
+      <c r="C40" s="17" t="inlineStr">
+        <is>
+          <t>Date Error</t>
         </is>
       </c>
     </row>
@@ -1266,9 +1266,9 @@
           <t>CMAU6652119</t>
         </is>
       </c>
-      <c r="C41" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2061</t>
+      <c r="C41" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1283,9 +1283,9 @@
           <t>TXGU6695032</t>
         </is>
       </c>
-      <c r="C42" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2062</t>
+      <c r="C42" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1300,9 +1300,9 @@
           <t>TCNU4397838</t>
         </is>
       </c>
-      <c r="C43" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2063</t>
+      <c r="C43" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1317,9 +1317,9 @@
           <t>FCIU8788223</t>
         </is>
       </c>
-      <c r="C44" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2064</t>
+      <c r="C44" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1334,9 +1334,9 @@
           <t>CMAU8671334</t>
         </is>
       </c>
-      <c r="C45" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2065</t>
+      <c r="C45" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1351,9 +1351,9 @@
           <t>APHU7074378</t>
         </is>
       </c>
-      <c r="C46" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2066</t>
+      <c r="C46" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1368,9 +1368,9 @@
           <t>TCNU4690511</t>
         </is>
       </c>
-      <c r="C47" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2067</t>
+      <c r="C47" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1385,9 +1385,9 @@
           <t>CMAU4822556</t>
         </is>
       </c>
-      <c r="C48" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2068</t>
+      <c r="C48" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1402,9 +1402,9 @@
           <t xml:space="preserve">CMAU6345370 </t>
         </is>
       </c>
-      <c r="C49" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2069</t>
+      <c r="C49" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1419,9 +1419,9 @@
           <t>CMAU9164252</t>
         </is>
       </c>
-      <c r="C50" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2070</t>
+      <c r="C50" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1436,9 +1436,9 @@
           <t>CMAU4361897</t>
         </is>
       </c>
-      <c r="C51" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2071</t>
+      <c r="C51" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1453,9 +1453,9 @@
           <t>CMAU4630105</t>
         </is>
       </c>
-      <c r="C52" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2072</t>
+      <c r="C52" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1470,9 +1470,9 @@
           <t>FSCU7131151</t>
         </is>
       </c>
-      <c r="C53" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2073</t>
+      <c r="C53" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1487,9 +1487,9 @@
           <t>APHU6321093</t>
         </is>
       </c>
-      <c r="C54" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2074</t>
+      <c r="C54" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1504,9 +1504,9 @@
           <t>CMAU0260851</t>
         </is>
       </c>
-      <c r="C55" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2075</t>
+      <c r="C55" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1521,9 +1521,9 @@
           <t>TGBU4169186</t>
         </is>
       </c>
-      <c r="C56" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2076</t>
+      <c r="C56" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1538,9 +1538,9 @@
           <t>APHU7270597</t>
         </is>
       </c>
-      <c r="C57" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2077</t>
+      <c r="C57" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1555,9 +1555,9 @@
           <t>TCNU1036512</t>
         </is>
       </c>
-      <c r="C58" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2078</t>
+      <c r="C58" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -1572,9 +1572,9 @@
           <t>TCLU8915814</t>
         </is>
       </c>
-      <c r="C59" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2079</t>
+      <c r="C59" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -1589,9 +1589,9 @@
           <t>APHU6367432</t>
         </is>
       </c>
-      <c r="C60" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2080</t>
+      <c r="C60" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -1606,9 +1606,9 @@
           <t>BEAU4009390</t>
         </is>
       </c>
-      <c r="C61" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2081</t>
+      <c r="C61" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -1623,9 +1623,9 @@
           <t>BEAU4125298</t>
         </is>
       </c>
-      <c r="C62" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2082</t>
+      <c r="C62" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -1640,9 +1640,9 @@
           <t>BEAU5955432</t>
         </is>
       </c>
-      <c r="C63" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2083</t>
+      <c r="C63" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -1657,9 +1657,9 @@
           <t>CAIU8925396</t>
         </is>
       </c>
-      <c r="C64" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2084</t>
+      <c r="C64" s="18" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
         </is>
       </c>
     </row>
@@ -1674,9 +1674,9 @@
           <t>CAIU9257178</t>
         </is>
       </c>
-      <c r="C65" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2085</t>
+      <c r="C65" s="18" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
         </is>
       </c>
     </row>
@@ -1691,9 +1691,9 @@
           <t>DFSU6935165</t>
         </is>
       </c>
-      <c r="C66" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2086</t>
+      <c r="C66" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -1708,9 +1708,9 @@
           <t>ECMU9870539</t>
         </is>
       </c>
-      <c r="C67" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2087</t>
+      <c r="C67" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -1725,9 +1725,9 @@
           <t>FFAU4290493</t>
         </is>
       </c>
-      <c r="C68" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2088</t>
+      <c r="C68" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -1742,9 +1742,9 @@
           <t>FCIU8248781</t>
         </is>
       </c>
-      <c r="C69" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2089</t>
+      <c r="C69" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -1759,9 +1759,9 @@
           <t>GESU5876310</t>
         </is>
       </c>
-      <c r="C70" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2090</t>
+      <c r="C70" s="18" t="inlineStr">
+        <is>
+          <t>06/27/2022</t>
         </is>
       </c>
     </row>
@@ -1776,9 +1776,9 @@
           <t>CMAU5726794</t>
         </is>
       </c>
-      <c r="C71" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2091</t>
+      <c r="C71" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -1793,9 +1793,9 @@
           <t>CMAU5875885</t>
         </is>
       </c>
-      <c r="C72" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2092</t>
+      <c r="C72" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -1810,9 +1810,9 @@
           <t>TCKU6228690</t>
         </is>
       </c>
-      <c r="C73" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2093</t>
+      <c r="C73" s="18" t="inlineStr">
+        <is>
+          <t>07/08/2022</t>
         </is>
       </c>
     </row>
@@ -1946,9 +1946,9 @@
           <t>EGHU9449660</t>
         </is>
       </c>
-      <c r="C81" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2101</t>
+      <c r="C81" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1963,9 +1963,9 @@
           <t>EGHU8329891</t>
         </is>
       </c>
-      <c r="C82" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2102</t>
+      <c r="C82" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1980,9 +1980,9 @@
           <t>EGHU9229006</t>
         </is>
       </c>
-      <c r="C83" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2103</t>
+      <c r="C83" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -1997,9 +1997,9 @@
           <t>TCKU6099376</t>
         </is>
       </c>
-      <c r="C84" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2104</t>
+      <c r="C84" s="18" t="inlineStr">
+        <is>
+          <t>06/26/2022</t>
         </is>
       </c>
     </row>
@@ -2014,9 +2014,9 @@
           <t>TCNU3811162</t>
         </is>
       </c>
-      <c r="C85" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2105</t>
+      <c r="C85" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2031,9 +2031,9 @@
           <t>TCNU6796800</t>
         </is>
       </c>
-      <c r="C86" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2106</t>
+      <c r="C86" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2048,9 +2048,9 @@
           <t>EITU1589389</t>
         </is>
       </c>
-      <c r="C87" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2107</t>
+      <c r="C87" s="18" t="inlineStr">
+        <is>
+          <t>06/26/2022</t>
         </is>
       </c>
     </row>
@@ -2065,9 +2065,9 @@
           <t>DRYU9855186</t>
         </is>
       </c>
-      <c r="C88" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2108</t>
+      <c r="C88" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2082,9 +2082,9 @@
           <t>FCIU9542189</t>
         </is>
       </c>
-      <c r="C89" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2109</t>
+      <c r="C89" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2099,9 +2099,9 @@
           <t>TCKU6124078</t>
         </is>
       </c>
-      <c r="C90" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2110</t>
+      <c r="C90" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2116,9 +2116,9 @@
           <t>TEMU6269179</t>
         </is>
       </c>
-      <c r="C91" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2111</t>
+      <c r="C91" s="18" t="inlineStr">
+        <is>
+          <t>06/26/2022</t>
         </is>
       </c>
     </row>
@@ -2133,9 +2133,9 @@
           <t>BSIU9250986</t>
         </is>
       </c>
-      <c r="C92" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2112</t>
+      <c r="C92" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2150,9 +2150,9 @@
           <t>EITU1742327</t>
         </is>
       </c>
-      <c r="C93" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2113</t>
+      <c r="C93" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2167,9 +2167,9 @@
           <t>TGBU4491000</t>
         </is>
       </c>
-      <c r="C94" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2114</t>
+      <c r="C94" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2184,9 +2184,9 @@
           <t>EGSU9166935</t>
         </is>
       </c>
-      <c r="C95" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2115</t>
+      <c r="C95" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2201,9 +2201,9 @@
           <t>BMOU5001758</t>
         </is>
       </c>
-      <c r="C96" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2116</t>
+      <c r="C96" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2218,9 +2218,9 @@
           <t>EISU9228537</t>
         </is>
       </c>
-      <c r="C97" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2117</t>
+      <c r="C97" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2235,9 +2235,9 @@
           <t>EGHU9483535</t>
         </is>
       </c>
-      <c r="C98" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2118</t>
+      <c r="C98" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2252,9 +2252,9 @@
           <t>TGBU6912433</t>
         </is>
       </c>
-      <c r="C99" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2119</t>
+      <c r="C99" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2269,9 +2269,9 @@
           <t>TCLU4970310</t>
         </is>
       </c>
-      <c r="C100" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2120</t>
+      <c r="C100" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2286,9 +2286,9 @@
           <t>DRYU9132309</t>
         </is>
       </c>
-      <c r="C101" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2121</t>
+      <c r="C101" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2303,9 +2303,9 @@
           <t>EITU9071631</t>
         </is>
       </c>
-      <c r="C102" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2122</t>
+      <c r="C102" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2320,9 +2320,9 @@
           <t>BEAU6310783</t>
         </is>
       </c>
-      <c r="C103" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2123</t>
+      <c r="C103" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2337,9 +2337,9 @@
           <t>MAGU5417922</t>
         </is>
       </c>
-      <c r="C104" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2124</t>
+      <c r="C104" s="18" t="inlineStr">
+        <is>
+          <t>06/30/2022</t>
         </is>
       </c>
     </row>
@@ -2354,9 +2354,9 @@
           <t>TGBU4523160</t>
         </is>
       </c>
-      <c r="C105" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2125</t>
+      <c r="C105" s="18" t="inlineStr">
+        <is>
+          <t>07/08/2022</t>
         </is>
       </c>
     </row>
@@ -2371,9 +2371,9 @@
           <t>EGHU9084664</t>
         </is>
       </c>
-      <c r="C106" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2126</t>
+      <c r="C106" s="18" t="inlineStr">
+        <is>
+          <t>06/30/2022</t>
         </is>
       </c>
     </row>
@@ -2388,9 +2388,9 @@
           <t>EMCU8546905</t>
         </is>
       </c>
-      <c r="C107" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2127</t>
+      <c r="C107" s="18" t="inlineStr">
+        <is>
+          <t>07/08/2022</t>
         </is>
       </c>
     </row>
@@ -2405,9 +2405,9 @@
           <t>EMCU8209653</t>
         </is>
       </c>
-      <c r="C108" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2128</t>
+      <c r="C108" s="18" t="inlineStr">
+        <is>
+          <t>07/08/2022</t>
         </is>
       </c>
     </row>
@@ -2558,9 +2558,9 @@
           <t>NYKU0725022</t>
         </is>
       </c>
-      <c r="C117" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2137</t>
+      <c r="C117" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2575,9 +2575,9 @@
           <t>GCXU5243011</t>
         </is>
       </c>
-      <c r="C118" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2138</t>
+      <c r="C118" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2592,9 +2592,9 @@
           <t>KSSU1004095</t>
         </is>
       </c>
-      <c r="C119" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2139</t>
+      <c r="C119" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2609,9 +2609,9 @@
           <t>KKFU8086626</t>
         </is>
       </c>
-      <c r="C120" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2140</t>
+      <c r="C120" s="18" t="inlineStr">
+        <is>
+          <t>07/13/2022</t>
         </is>
       </c>
     </row>
@@ -2626,9 +2626,9 @@
           <t>TGHU6504140</t>
         </is>
       </c>
-      <c r="C121" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2141</t>
+      <c r="C121" s="18" t="inlineStr">
+        <is>
+          <t>08/05/2022</t>
         </is>
       </c>
     </row>
@@ -2643,9 +2643,9 @@
           <t>ONEU0006854</t>
         </is>
       </c>
-      <c r="C122" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2142</t>
+      <c r="C122" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2660,9 +2660,9 @@
           <t>TRHU4017274</t>
         </is>
       </c>
-      <c r="C123" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2143</t>
+      <c r="C123" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2677,9 +2677,9 @@
           <t>TCNU7076512</t>
         </is>
       </c>
-      <c r="C124" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2144</t>
+      <c r="C124" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2694,9 +2694,9 @@
           <t>NYKU0811434</t>
         </is>
       </c>
-      <c r="C125" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2145</t>
+      <c r="C125" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2711,9 +2711,9 @@
           <t>CAIU9538160</t>
         </is>
       </c>
-      <c r="C126" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2146</t>
+      <c r="C126" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2728,9 +2728,9 @@
           <t>TEMU7202776</t>
         </is>
       </c>
-      <c r="C127" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2147</t>
+      <c r="C127" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2745,9 +2745,9 @@
           <t>HLXU8136823</t>
         </is>
       </c>
-      <c r="C128" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2148</t>
+      <c r="C128" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2762,9 +2762,9 @@
           <t>TCLU1790145</t>
         </is>
       </c>
-      <c r="C129" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2149</t>
+      <c r="C129" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2779,9 +2779,9 @@
           <t xml:space="preserve">TCNU8395005	</t>
         </is>
       </c>
-      <c r="C130" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2150</t>
+      <c r="C130" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2841,9 +2841,9 @@
           <t>CMAU0459057</t>
         </is>
       </c>
-      <c r="C2" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2022</t>
+      <c r="C2" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2858,9 +2858,9 @@
           <t>CMAU1999430</t>
         </is>
       </c>
-      <c r="C3" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2023</t>
+      <c r="C3" s="17" t="inlineStr">
+        <is>
+          <t>Date Error</t>
         </is>
       </c>
     </row>
@@ -2875,9 +2875,9 @@
           <t>TEMU1001882</t>
         </is>
       </c>
-      <c r="C4" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2024</t>
+      <c r="C4" s="17" t="inlineStr">
+        <is>
+          <t>Date Error</t>
         </is>
       </c>
     </row>
@@ -2892,9 +2892,9 @@
           <t>CMAU3124870</t>
         </is>
       </c>
-      <c r="C5" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2025</t>
+      <c r="C5" s="18" t="inlineStr">
+        <is>
+          <t>07/06/2022</t>
         </is>
       </c>
     </row>
@@ -2909,9 +2909,9 @@
           <t>CMAU1271001</t>
         </is>
       </c>
-      <c r="C6" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2026</t>
+      <c r="C6" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -2926,9 +2926,9 @@
           <t>CMAU1084274</t>
         </is>
       </c>
-      <c r="C7" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2027</t>
+      <c r="C7" s="18" t="inlineStr">
+        <is>
+          <t>07/07/2022</t>
         </is>
       </c>
     </row>
@@ -2943,9 +2943,9 @@
           <t>TLLU2340963</t>
         </is>
       </c>
-      <c r="C8" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2028</t>
+      <c r="C8" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -2960,9 +2960,9 @@
           <t>CMAU0786511</t>
         </is>
       </c>
-      <c r="C9" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2029</t>
+      <c r="C9" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -2977,9 +2977,9 @@
           <t>TGHU9843127</t>
         </is>
       </c>
-      <c r="C10" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2030</t>
+      <c r="C10" s="18" t="inlineStr">
+        <is>
+          <t>07/06/2022</t>
         </is>
       </c>
     </row>
@@ -2994,9 +2994,9 @@
           <t>BMOU2183772</t>
         </is>
       </c>
-      <c r="C11" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2031</t>
+      <c r="C11" s="17" t="inlineStr">
+        <is>
+          <t>Date Error</t>
         </is>
       </c>
     </row>
@@ -3011,9 +3011,9 @@
           <t>BMOU2182267</t>
         </is>
       </c>
-      <c r="C12" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2032</t>
+      <c r="C12" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3028,9 +3028,9 @@
           <t>TEMU2454266</t>
         </is>
       </c>
-      <c r="C13" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2033</t>
+      <c r="C13" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3045,9 +3045,9 @@
           <t>CMAU0615186</t>
         </is>
       </c>
-      <c r="C14" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2034</t>
+      <c r="C14" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3062,9 +3062,9 @@
           <t>CMAU1671749</t>
         </is>
       </c>
-      <c r="C15" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2035</t>
+      <c r="C15" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3079,9 +3079,9 @@
           <t>FWRU0143517</t>
         </is>
       </c>
-      <c r="C16" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2036</t>
+      <c r="C16" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3096,9 +3096,9 @@
           <t>TCLU9637873</t>
         </is>
       </c>
-      <c r="C17" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2037</t>
+      <c r="C17" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -3113,9 +3113,9 @@
           <t>TRHU6017442</t>
         </is>
       </c>
-      <c r="C18" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2038</t>
+      <c r="C18" s="18" t="inlineStr">
+        <is>
+          <t>07/17/2022</t>
         </is>
       </c>
     </row>
@@ -3130,9 +3130,9 @@
           <t>FCIU9357391</t>
         </is>
       </c>
-      <c r="C19" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2039</t>
+      <c r="C19" s="18" t="inlineStr">
+        <is>
+          <t>07/29/2022</t>
         </is>
       </c>
     </row>
@@ -3147,9 +3147,9 @@
           <t>CMAU7146898</t>
         </is>
       </c>
-      <c r="C20" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2040</t>
+      <c r="C20" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3164,9 +3164,9 @@
           <t>CMAU5249433</t>
         </is>
       </c>
-      <c r="C21" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2041</t>
+      <c r="C21" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3181,9 +3181,9 @@
           <t>CMAU5905357</t>
         </is>
       </c>
-      <c r="C22" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2042</t>
+      <c r="C22" s="18" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
         </is>
       </c>
     </row>
@@ -3198,9 +3198,9 @@
           <t>TGHU3892802</t>
         </is>
       </c>
-      <c r="C23" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2043</t>
+      <c r="C23" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3215,9 +3215,9 @@
           <t>TGHU0157086</t>
         </is>
       </c>
-      <c r="C24" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2044</t>
+      <c r="C24" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3232,9 +3232,9 @@
           <t>APZU3448600</t>
         </is>
       </c>
-      <c r="C25" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2045</t>
+      <c r="C25" s="18" t="inlineStr">
+        <is>
+          <t>07/05/2022</t>
         </is>
       </c>
     </row>
@@ -3249,9 +3249,9 @@
           <t>APZU3431438</t>
         </is>
       </c>
-      <c r="C26" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2046</t>
+      <c r="C26" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3266,9 +3266,9 @@
           <t>MAGU5474162</t>
         </is>
       </c>
-      <c r="C27" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2047</t>
+      <c r="C27" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3283,9 +3283,9 @@
           <t>TRLU6706305</t>
         </is>
       </c>
-      <c r="C28" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2048</t>
+      <c r="C28" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3300,9 +3300,9 @@
           <t>FCIU8749361</t>
         </is>
       </c>
-      <c r="C29" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2049</t>
+      <c r="C29" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3317,9 +3317,9 @@
           <t>CMAU5084396</t>
         </is>
       </c>
-      <c r="C30" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2050</t>
+      <c r="C30" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3334,9 +3334,9 @@
           <t>TCKU6331265</t>
         </is>
       </c>
-      <c r="C31" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2051</t>
+      <c r="C31" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3351,9 +3351,9 @@
           <t>TCNU2838050</t>
         </is>
       </c>
-      <c r="C32" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2052</t>
+      <c r="C32" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3368,9 +3368,9 @@
           <t>TEMU6960719</t>
         </is>
       </c>
-      <c r="C33" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2053</t>
+      <c r="C33" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3385,9 +3385,9 @@
           <t>TLLU4514961</t>
         </is>
       </c>
-      <c r="C34" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2054</t>
+      <c r="C34" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3402,9 +3402,9 @@
           <t>CMAU0594020</t>
         </is>
       </c>
-      <c r="C35" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2055</t>
+      <c r="C35" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3419,9 +3419,9 @@
           <t>CMAU1317484</t>
         </is>
       </c>
-      <c r="C36" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2056</t>
+      <c r="C36" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3436,9 +3436,9 @@
           <t>TCLU9647362</t>
         </is>
       </c>
-      <c r="C37" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2057</t>
+      <c r="C37" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3453,9 +3453,9 @@
           <t>TRHU8141283</t>
         </is>
       </c>
-      <c r="C38" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2058</t>
+      <c r="C38" s="18" t="inlineStr">
+        <is>
+          <t>08/04/2022</t>
         </is>
       </c>
     </row>
@@ -3470,9 +3470,9 @@
           <t>TCLU8644395</t>
         </is>
       </c>
-      <c r="C39" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2059</t>
+      <c r="C39" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3487,9 +3487,9 @@
           <t>JXLU7831639</t>
         </is>
       </c>
-      <c r="C40" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2060</t>
+      <c r="C40" s="17" t="inlineStr">
+        <is>
+          <t>Date Error</t>
         </is>
       </c>
     </row>
@@ -3504,9 +3504,9 @@
           <t>CMAU6652119</t>
         </is>
       </c>
-      <c r="C41" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2061</t>
+      <c r="C41" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3521,9 +3521,9 @@
           <t>TXGU6695032</t>
         </is>
       </c>
-      <c r="C42" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2062</t>
+      <c r="C42" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3538,9 +3538,9 @@
           <t>TCNU4397838</t>
         </is>
       </c>
-      <c r="C43" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2063</t>
+      <c r="C43" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3555,9 +3555,9 @@
           <t>FCIU8788223</t>
         </is>
       </c>
-      <c r="C44" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2064</t>
+      <c r="C44" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3572,9 +3572,9 @@
           <t>CMAU8671334</t>
         </is>
       </c>
-      <c r="C45" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2065</t>
+      <c r="C45" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3589,9 +3589,9 @@
           <t>APHU7074378</t>
         </is>
       </c>
-      <c r="C46" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2066</t>
+      <c r="C46" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3606,9 +3606,9 @@
           <t>TCNU4690511</t>
         </is>
       </c>
-      <c r="C47" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2067</t>
+      <c r="C47" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3623,9 +3623,9 @@
           <t>CMAU4822556</t>
         </is>
       </c>
-      <c r="C48" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2068</t>
+      <c r="C48" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3640,9 +3640,9 @@
           <t xml:space="preserve">CMAU6345370 </t>
         </is>
       </c>
-      <c r="C49" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2069</t>
+      <c r="C49" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3657,9 +3657,9 @@
           <t>CMAU9164252</t>
         </is>
       </c>
-      <c r="C50" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2070</t>
+      <c r="C50" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3674,9 +3674,9 @@
           <t>CMAU4361897</t>
         </is>
       </c>
-      <c r="C51" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2071</t>
+      <c r="C51" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3691,9 +3691,9 @@
           <t>CMAU4630105</t>
         </is>
       </c>
-      <c r="C52" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2072</t>
+      <c r="C52" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3708,9 +3708,9 @@
           <t>FSCU7131151</t>
         </is>
       </c>
-      <c r="C53" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2073</t>
+      <c r="C53" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3725,9 +3725,9 @@
           <t>APHU6321093</t>
         </is>
       </c>
-      <c r="C54" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2074</t>
+      <c r="C54" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3742,9 +3742,9 @@
           <t>CMAU0260851</t>
         </is>
       </c>
-      <c r="C55" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2075</t>
+      <c r="C55" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -3759,9 +3759,9 @@
           <t>TGBU4169186</t>
         </is>
       </c>
-      <c r="C56" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2076</t>
+      <c r="C56" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3776,9 +3776,9 @@
           <t>APHU7270597</t>
         </is>
       </c>
-      <c r="C57" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2077</t>
+      <c r="C57" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3793,9 +3793,9 @@
           <t>TCNU1036512</t>
         </is>
       </c>
-      <c r="C58" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2078</t>
+      <c r="C58" s="18" t="inlineStr">
+        <is>
+          <t>06/23/2022</t>
         </is>
       </c>
     </row>
@@ -3810,9 +3810,9 @@
           <t>TCLU8915814</t>
         </is>
       </c>
-      <c r="C59" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2079</t>
+      <c r="C59" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -3827,9 +3827,9 @@
           <t>APHU6367432</t>
         </is>
       </c>
-      <c r="C60" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2080</t>
+      <c r="C60" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -3844,9 +3844,9 @@
           <t>BEAU4009390</t>
         </is>
       </c>
-      <c r="C61" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2081</t>
+      <c r="C61" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -3861,9 +3861,9 @@
           <t>BEAU4125298</t>
         </is>
       </c>
-      <c r="C62" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2082</t>
+      <c r="C62" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -3878,9 +3878,9 @@
           <t>BEAU5955432</t>
         </is>
       </c>
-      <c r="C63" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2083</t>
+      <c r="C63" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -3895,9 +3895,9 @@
           <t>CAIU8925396</t>
         </is>
       </c>
-      <c r="C64" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2084</t>
+      <c r="C64" s="18" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
         </is>
       </c>
     </row>
@@ -3912,9 +3912,9 @@
           <t>CAIU9257178</t>
         </is>
       </c>
-      <c r="C65" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2085</t>
+      <c r="C65" s="18" t="inlineStr">
+        <is>
+          <t>07/01/2022</t>
         </is>
       </c>
     </row>
@@ -3929,9 +3929,9 @@
           <t>DFSU6935165</t>
         </is>
       </c>
-      <c r="C66" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2086</t>
+      <c r="C66" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -3946,9 +3946,9 @@
           <t>ECMU9870539</t>
         </is>
       </c>
-      <c r="C67" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2087</t>
+      <c r="C67" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -3963,9 +3963,9 @@
           <t>FFAU4290493</t>
         </is>
       </c>
-      <c r="C68" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2088</t>
+      <c r="C68" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -3980,9 +3980,9 @@
           <t>FCIU8248781</t>
         </is>
       </c>
-      <c r="C69" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2089</t>
+      <c r="C69" s="18" t="inlineStr">
+        <is>
+          <t>07/25/2022</t>
         </is>
       </c>
     </row>
@@ -3997,9 +3997,9 @@
           <t>GESU5876310</t>
         </is>
       </c>
-      <c r="C70" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2090</t>
+      <c r="C70" s="18" t="inlineStr">
+        <is>
+          <t>06/27/2022</t>
         </is>
       </c>
     </row>
@@ -4014,9 +4014,9 @@
           <t>CMAU5726794</t>
         </is>
       </c>
-      <c r="C71" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2091</t>
+      <c r="C71" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -4031,9 +4031,9 @@
           <t>CMAU5875885</t>
         </is>
       </c>
-      <c r="C72" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2092</t>
+      <c r="C72" s="18" t="inlineStr">
+        <is>
+          <t>07/03/2022</t>
         </is>
       </c>
     </row>
@@ -4048,9 +4048,9 @@
           <t>TCKU6228690</t>
         </is>
       </c>
-      <c r="C73" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2093</t>
+      <c r="C73" s="18" t="inlineStr">
+        <is>
+          <t>07/08/2022</t>
         </is>
       </c>
     </row>
@@ -4184,9 +4184,9 @@
           <t>EGHU9449660</t>
         </is>
       </c>
-      <c r="C81" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2101</t>
+      <c r="C81" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4201,9 +4201,9 @@
           <t>EGHU8329891</t>
         </is>
       </c>
-      <c r="C82" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2102</t>
+      <c r="C82" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4218,9 +4218,9 @@
           <t>EGHU9229006</t>
         </is>
       </c>
-      <c r="C83" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2103</t>
+      <c r="C83" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4235,9 +4235,9 @@
           <t>TCKU6099376</t>
         </is>
       </c>
-      <c r="C84" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2104</t>
+      <c r="C84" s="18" t="inlineStr">
+        <is>
+          <t>06/26/2022</t>
         </is>
       </c>
     </row>
@@ -4252,9 +4252,9 @@
           <t>TCNU3811162</t>
         </is>
       </c>
-      <c r="C85" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2105</t>
+      <c r="C85" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4269,9 +4269,9 @@
           <t>TCNU6796800</t>
         </is>
       </c>
-      <c r="C86" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2106</t>
+      <c r="C86" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4286,9 +4286,9 @@
           <t>EITU1589389</t>
         </is>
       </c>
-      <c r="C87" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2107</t>
+      <c r="C87" s="18" t="inlineStr">
+        <is>
+          <t>06/26/2022</t>
         </is>
       </c>
     </row>
@@ -4303,9 +4303,9 @@
           <t>DRYU9855186</t>
         </is>
       </c>
-      <c r="C88" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2108</t>
+      <c r="C88" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4320,9 +4320,9 @@
           <t>FCIU9542189</t>
         </is>
       </c>
-      <c r="C89" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2109</t>
+      <c r="C89" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4337,9 +4337,9 @@
           <t>TCKU6124078</t>
         </is>
       </c>
-      <c r="C90" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2110</t>
+      <c r="C90" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4354,9 +4354,9 @@
           <t>TEMU6269179</t>
         </is>
       </c>
-      <c r="C91" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2111</t>
+      <c r="C91" s="18" t="inlineStr">
+        <is>
+          <t>06/26/2022</t>
         </is>
       </c>
     </row>
@@ -4371,9 +4371,9 @@
           <t>BSIU9250986</t>
         </is>
       </c>
-      <c r="C92" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2112</t>
+      <c r="C92" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4388,9 +4388,9 @@
           <t>EITU1742327</t>
         </is>
       </c>
-      <c r="C93" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2113</t>
+      <c r="C93" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4405,9 +4405,9 @@
           <t>TGBU4491000</t>
         </is>
       </c>
-      <c r="C94" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2114</t>
+      <c r="C94" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4422,9 +4422,9 @@
           <t>EGSU9166935</t>
         </is>
       </c>
-      <c r="C95" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2115</t>
+      <c r="C95" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4439,9 +4439,9 @@
           <t>BMOU5001758</t>
         </is>
       </c>
-      <c r="C96" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2116</t>
+      <c r="C96" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4456,9 +4456,9 @@
           <t>EISU9228537</t>
         </is>
       </c>
-      <c r="C97" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2117</t>
+      <c r="C97" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4473,9 +4473,9 @@
           <t>EGHU9483535</t>
         </is>
       </c>
-      <c r="C98" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2118</t>
+      <c r="C98" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4490,9 +4490,9 @@
           <t>TGBU6912433</t>
         </is>
       </c>
-      <c r="C99" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2119</t>
+      <c r="C99" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4507,9 +4507,9 @@
           <t>TCLU4970310</t>
         </is>
       </c>
-      <c r="C100" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2120</t>
+      <c r="C100" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4524,9 +4524,9 @@
           <t>DRYU9132309</t>
         </is>
       </c>
-      <c r="C101" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2121</t>
+      <c r="C101" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4541,9 +4541,9 @@
           <t>EITU9071631</t>
         </is>
       </c>
-      <c r="C102" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2122</t>
+      <c r="C102" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4558,9 +4558,9 @@
           <t>BEAU6310783</t>
         </is>
       </c>
-      <c r="C103" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2123</t>
+      <c r="C103" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4575,9 +4575,9 @@
           <t>MAGU5417922</t>
         </is>
       </c>
-      <c r="C104" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2124</t>
+      <c r="C104" s="18" t="inlineStr">
+        <is>
+          <t>06/30/2022</t>
         </is>
       </c>
     </row>
@@ -4592,9 +4592,9 @@
           <t>TGBU4523160</t>
         </is>
       </c>
-      <c r="C105" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2125</t>
+      <c r="C105" s="18" t="inlineStr">
+        <is>
+          <t>07/08/2022</t>
         </is>
       </c>
     </row>
@@ -4609,9 +4609,9 @@
           <t>EGHU9084664</t>
         </is>
       </c>
-      <c r="C106" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2126</t>
+      <c r="C106" s="18" t="inlineStr">
+        <is>
+          <t>06/30/2022</t>
         </is>
       </c>
     </row>
@@ -4626,9 +4626,9 @@
           <t>EMCU8546905</t>
         </is>
       </c>
-      <c r="C107" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2127</t>
+      <c r="C107" s="18" t="inlineStr">
+        <is>
+          <t>07/08/2022</t>
         </is>
       </c>
     </row>
@@ -4643,9 +4643,9 @@
           <t>EMCU8209653</t>
         </is>
       </c>
-      <c r="C108" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2128</t>
+      <c r="C108" s="18" t="inlineStr">
+        <is>
+          <t>07/08/2022</t>
         </is>
       </c>
     </row>
@@ -4796,9 +4796,9 @@
           <t>NYKU0725022</t>
         </is>
       </c>
-      <c r="C117" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2137</t>
+      <c r="C117" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4813,9 +4813,9 @@
           <t>GCXU5243011</t>
         </is>
       </c>
-      <c r="C118" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2138</t>
+      <c r="C118" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4830,9 +4830,9 @@
           <t>KSSU1004095</t>
         </is>
       </c>
-      <c r="C119" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2139</t>
+      <c r="C119" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4847,9 +4847,9 @@
           <t>KKFU8086626</t>
         </is>
       </c>
-      <c r="C120" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2140</t>
+      <c r="C120" s="18" t="inlineStr">
+        <is>
+          <t>07/13/2022</t>
         </is>
       </c>
     </row>
@@ -4864,9 +4864,9 @@
           <t>TGHU6504140</t>
         </is>
       </c>
-      <c r="C121" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2141</t>
+      <c r="C121" s="18" t="inlineStr">
+        <is>
+          <t>08/05/2022</t>
         </is>
       </c>
     </row>
@@ -4881,9 +4881,9 @@
           <t>ONEU0006854</t>
         </is>
       </c>
-      <c r="C122" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2142</t>
+      <c r="C122" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4898,9 +4898,9 @@
           <t>TRHU4017274</t>
         </is>
       </c>
-      <c r="C123" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2143</t>
+      <c r="C123" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4915,9 +4915,9 @@
           <t>TCNU7076512</t>
         </is>
       </c>
-      <c r="C124" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2144</t>
+      <c r="C124" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4932,9 +4932,9 @@
           <t>NYKU0811434</t>
         </is>
       </c>
-      <c r="C125" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2145</t>
+      <c r="C125" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4949,9 +4949,9 @@
           <t>CAIU9538160</t>
         </is>
       </c>
-      <c r="C126" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2146</t>
+      <c r="C126" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4966,9 +4966,9 @@
           <t>TEMU7202776</t>
         </is>
       </c>
-      <c r="C127" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2147</t>
+      <c r="C127" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -4983,9 +4983,9 @@
           <t>HLXU8136823</t>
         </is>
       </c>
-      <c r="C128" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2148</t>
+      <c r="C128" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -5000,9 +5000,9 @@
           <t>TCLU1790145</t>
         </is>
       </c>
-      <c r="C129" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2149</t>
+      <c r="C129" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>
@@ -5017,9 +5017,9 @@
           <t xml:space="preserve">TCNU8395005	</t>
         </is>
       </c>
-      <c r="C130" s="15" t="inlineStr">
-        <is>
-          <t>06/21/2150</t>
+      <c r="C130" s="16" t="inlineStr">
+        <is>
+          <t>arrived</t>
         </is>
       </c>
     </row>

</xml_diff>